<commit_message>
Now pops up warning and uses macro inside project
</commit_message>
<xml_diff>
--- a/Mappe2.xlsx
+++ b/Mappe2.xlsx
@@ -2,6 +2,11 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet name="Beispiel" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
@@ -10,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="133">
   <si>
     <t>EFKey</t>
   </si>
@@ -415,26 +420,41 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS" numFmtId="166"/>
-    <numFmt formatCode="HH:MM:SS" numFmtId="167"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="4">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
-  <fills count="1">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -442,818 +462,493 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="164">
-</xf>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="164" xfId="0"/>
-    <xf numFmtId="165" xfId="0"/>
-    <xf numFmtId="166" xfId="0"/>
-    <xf numFmtId="167" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <cols>
-    <col min="1" max="1024" width="15"/>
-    <col min="2" max="1024" width="15"/>
-    <col min="3" max="1024" width="15"/>
-    <col min="4" max="1024" width="15"/>
-    <col min="5" max="1024" width="15"/>
-    <col min="6" max="1024" width="15"/>
-    <col min="7" max="1024" width="15"/>
-    <col min="8" max="1024" width="15"/>
-    <col min="9" max="1024" width="15"/>
-    <col min="10" max="1024" width="15"/>
-    <col min="11" max="1024" width="15"/>
-    <col min="12" max="1024" width="15"/>
-    <col min="13" max="1024" width="15"/>
-    <col min="14" max="1024" width="15"/>
-    <col min="15" max="1024" width="15"/>
-    <col min="16" max="1024" width="15"/>
-    <col min="17" max="1024" width="15"/>
-    <col min="18" max="1024" width="15"/>
-    <col min="19" max="1024" width="15"/>
-    <col min="20" max="1024" width="15"/>
-    <col min="21" max="1024" width="15"/>
-    <col min="22" max="1024" width="15"/>
-    <col min="23" max="1024" width="15"/>
-    <col min="24" max="1024" width="15"/>
-    <col min="25" max="1024" width="15"/>
-    <col min="26" max="1024" width="15"/>
-    <col min="27" max="1024" width="15"/>
-    <col min="28" max="1024" width="15"/>
-    <col min="29" max="1024" width="15"/>
-    <col min="30" max="1024" width="15"/>
-    <col min="31" max="1024" width="15"/>
-    <col min="32" max="1024" width="15"/>
-    <col min="33" max="1024" width="15"/>
-    <col min="34" max="1024" width="15"/>
-    <col min="35" max="1024" width="15"/>
-    <col min="36" max="1024" width="15"/>
-    <col min="37" max="1024" width="15"/>
-    <col min="38" max="1024" width="15"/>
-    <col min="39" max="1024" width="15"/>
-    <col min="40" max="1024" width="15"/>
-    <col min="41" max="1024" width="15"/>
-    <col min="42" max="1024" width="15"/>
-    <col min="43" max="1024" width="15"/>
-    <col min="44" max="1024" width="15"/>
-    <col min="45" max="1024" width="15"/>
-    <col min="46" max="1024" width="15"/>
-    <col min="47" max="1024" width="15"/>
-    <col min="48" max="1024" width="15"/>
-    <col min="49" max="1024" width="15"/>
-    <col min="50" max="1024" width="15"/>
-    <col min="51" max="1024" width="15"/>
-    <col min="52" max="1024" width="15"/>
-    <col min="53" max="1024" width="15"/>
-    <col min="54" max="1024" width="15"/>
-    <col min="55" max="1024" width="15"/>
-    <col min="56" max="1024" width="15"/>
-    <col min="57" max="1024" width="15"/>
-    <col min="58" max="1024" width="15"/>
-    <col min="59" max="1024" width="15"/>
-    <col min="60" max="1024" width="15"/>
-    <col min="61" max="1024" width="15"/>
-    <col min="62" max="1024" width="15"/>
-    <col min="63" max="1024" width="15"/>
-    <col min="64" max="1024" width="15"/>
-    <col min="65" max="1024" width="15"/>
-    <col min="66" max="1024" width="15"/>
-    <col min="67" max="1024" width="15"/>
-    <col min="68" max="1024" width="15"/>
-    <col min="69" max="1024" width="15"/>
-    <col min="70" max="1024" width="15"/>
-    <col min="71" max="1024" width="15"/>
-    <col min="72" max="1024" width="15"/>
-    <col min="73" max="1024" width="15"/>
-    <col min="74" max="1024" width="15"/>
-    <col min="75" max="1024" width="15"/>
-    <col min="76" max="1024" width="15"/>
-    <col min="77" max="1024" width="15"/>
-    <col min="78" max="1024" width="15"/>
-    <col min="79" max="1024" width="15"/>
-    <col min="80" max="1024" width="15"/>
-    <col min="81" max="1024" width="15"/>
-    <col min="82" max="1024" width="15"/>
-    <col min="83" max="1024" width="15"/>
-    <col min="84" max="1024" width="15"/>
-    <col min="85" max="1024" width="15"/>
-    <col min="86" max="1024" width="15"/>
-    <col min="87" max="1024" width="15"/>
-    <col min="88" max="1024" width="15"/>
-    <col min="89" max="1024" width="15"/>
-    <col min="90" max="1024" width="15"/>
-    <col min="91" max="1024" width="15"/>
-  </cols>
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:DM4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BA1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BB1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BC1" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BD1" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BE1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BF1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BG1" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BH1" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BI1" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BJ1" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BK1" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BL1" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BM1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BN1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BO1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BP1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BQ1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BR1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BS1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BT1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BU1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BV1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BW1" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BX1" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BY1" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="BZ1" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CA1" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CB1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CC1" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CD1" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CE1" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CF1" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CG1" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CH1" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CI1" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CJ1" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CK1" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CL1" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CM1" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CN1" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CO1" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CP1" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CQ1" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CR1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CS1" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CT1" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CU1" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CV1" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CW1" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CX1" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CY1" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="CZ1" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DA1" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DB1" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DC1" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DD1" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DE1" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DF1" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DG1" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DH1" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DI1" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DJ1" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DK1" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DL1" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DM1" s="0" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="0" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BA3" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BB3" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="BC3" t="s">
+      <c r="BC3" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="BD3" t="s">
+      <c r="BD3" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BE3" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="BF3" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="BH3" t="s">
+      <c r="BH3" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="BI3" t="s">
+      <c r="BI3" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="BJ3" t="s">
+      <c r="BJ3" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="BK3" t="s">
+      <c r="BK3" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="BM3" t="s">
+      <c r="BM3" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="0" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>16</v>
-      </c>
-      <c r="R5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" t="s">
-        <v>18</v>
-      </c>
-      <c r="T5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" t="s">
-        <v>20</v>
-      </c>
-      <c r="V5" t="s">
-        <v>21</v>
-      </c>
-      <c r="W5" t="s">
-        <v>22</v>
-      </c>
-      <c r="X5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>25</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>26</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>27</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>28</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>29</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>30</v>
-      </c>
-      <c r="BF5" t="s">
-        <v>31</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BH5" t="s">
-        <v>33</v>
-      </c>
-      <c r="BI5" t="s">
-        <v>34</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>35</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>36</v>
-      </c>
-      <c r="BL5" t="s">
-        <v>37</v>
-      </c>
-      <c r="BM5" t="s">
-        <v>38</v>
-      </c>
-      <c r="BN5" t="s">
-        <v>39</v>
-      </c>
-      <c r="BO5" t="s">
-        <v>40</v>
-      </c>
-      <c r="BP5" t="s">
-        <v>41</v>
-      </c>
-      <c r="BQ5" t="s">
-        <v>42</v>
-      </c>
-      <c r="BR5" t="s">
-        <v>43</v>
-      </c>
-      <c r="BS5" t="s">
-        <v>44</v>
-      </c>
-      <c r="BT5" t="s">
-        <v>45</v>
-      </c>
-      <c r="BU5" t="s">
-        <v>46</v>
-      </c>
-      <c r="BV5" t="s">
-        <v>47</v>
-      </c>
-      <c r="BW5" t="s">
-        <v>48</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>49</v>
-      </c>
-      <c r="BY5" t="s">
-        <v>50</v>
-      </c>
-      <c r="BZ5" t="s">
-        <v>51</v>
-      </c>
-      <c r="CA5" t="s">
-        <v>52</v>
-      </c>
-      <c r="CB5" t="s">
-        <v>53</v>
-      </c>
-      <c r="CC5" t="s">
-        <v>54</v>
-      </c>
-      <c r="CD5" t="s">
-        <v>55</v>
-      </c>
-      <c r="CE5" t="s">
-        <v>56</v>
-      </c>
-      <c r="CF5" t="s">
-        <v>57</v>
-      </c>
-      <c r="CG5" t="s">
-        <v>58</v>
-      </c>
-      <c r="CH5" t="s">
-        <v>59</v>
-      </c>
-      <c r="CI5" t="s">
-        <v>60</v>
-      </c>
-      <c r="CJ5" t="s">
-        <v>61</v>
-      </c>
-      <c r="CK5" t="s">
-        <v>62</v>
-      </c>
-      <c r="CL5" t="s">
-        <v>63</v>
-      </c>
-      <c r="CM5" t="s">
-        <v>64</v>
-      </c>
-      <c r="CN5" t="s">
-        <v>65</v>
-      </c>
-      <c r="CO5" t="s">
-        <v>66</v>
-      </c>
-      <c r="CP5" t="s">
-        <v>67</v>
-      </c>
-      <c r="CQ5" t="s">
-        <v>68</v>
-      </c>
-      <c r="CR5" t="s">
-        <v>69</v>
-      </c>
-      <c r="CS5" t="s">
-        <v>70</v>
-      </c>
-      <c r="CT5" t="s">
-        <v>71</v>
-      </c>
-      <c r="CU5" t="s">
-        <v>72</v>
-      </c>
-      <c r="CV5" t="s">
-        <v>73</v>
-      </c>
-      <c r="CW5" t="s">
-        <v>74</v>
-      </c>
-      <c r="CX5" t="s">
-        <v>75</v>
-      </c>
-      <c r="CY5" t="s">
-        <v>76</v>
-      </c>
-      <c r="CZ5" t="s">
-        <v>77</v>
-      </c>
-      <c r="DA5" t="s">
-        <v>78</v>
-      </c>
-      <c r="DB5" t="s">
-        <v>79</v>
-      </c>
-      <c r="DC5" t="s">
-        <v>80</v>
-      </c>
-      <c r="DD5" t="s">
-        <v>81</v>
-      </c>
-      <c r="DE5" t="s">
-        <v>82</v>
-      </c>
-      <c r="DF5" t="s">
-        <v>83</v>
-      </c>
-      <c r="DG5" t="s">
-        <v>84</v>
-      </c>
-      <c r="DH5" t="s">
-        <v>85</v>
-      </c>
-      <c r="DI5" t="s">
-        <v>86</v>
-      </c>
-      <c r="DJ5" t="s">
-        <v>87</v>
-      </c>
-      <c r="DK5" t="s">
-        <v>88</v>
-      </c>
-      <c r="DL5" t="s">
-        <v>89</v>
-      </c>
-      <c r="DM5" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Using pandas to write to excel instead of ogr
</commit_message>
<xml_diff>
--- a/Mappe2.xlsx
+++ b/Mappe2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="134">
   <si>
     <t>EFKey</t>
   </si>
@@ -293,6 +293,9 @@
     <t>2015-46-462</t>
   </si>
   <si>
+    <t>dfdf</t>
+  </si>
+  <si>
     <t>Schlag 1</t>
   </si>
   <si>
@@ -335,7 +338,7 @@
     <t>Privat</t>
   </si>
   <si>
-    <t>3</t>
+    <t>dfdfd</t>
   </si>
   <si>
     <t>Law, Blockschutt</t>
@@ -428,6 +431,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -487,8 +491,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,434 +520,440 @@
   <dimension ref="A1:DM4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="BA1" s="0" t="s">
+      <c r="BA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="BB1" s="0" t="s">
+      <c r="BB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="BC1" s="0" t="s">
+      <c r="BC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="BD1" s="0" t="s">
+      <c r="BD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="BE1" s="0" t="s">
+      <c r="BE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="BF1" s="0" t="s">
+      <c r="BF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="BG1" s="0" t="s">
+      <c r="BG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="BH1" s="0" t="s">
+      <c r="BH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="BI1" s="0" t="s">
+      <c r="BI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="BJ1" s="0" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="BK1" s="0" t="s">
+      <c r="BK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="BL1" s="0" t="s">
+      <c r="BL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BM1" s="0" t="s">
+      <c r="BM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="BN1" s="0" t="s">
+      <c r="BN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="BO1" s="0" t="s">
+      <c r="BO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BP1" s="0" t="s">
+      <c r="BP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="BQ1" s="0" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="BR1" s="0" t="s">
+      <c r="BR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="BS1" s="0" t="s">
+      <c r="BS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="BT1" s="0" t="s">
+      <c r="BT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BU1" s="0" t="s">
+      <c r="BU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BV1" s="0" t="s">
+      <c r="BV1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="BW1" s="0" t="s">
+      <c r="BW1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BX1" s="0" t="s">
+      <c r="BX1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BY1" s="0" t="s">
+      <c r="BY1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BZ1" s="0" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="CA1" s="0" t="s">
+      <c r="CA1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="CB1" s="0" t="s">
+      <c r="CB1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="CC1" s="0" t="s">
+      <c r="CC1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="CD1" s="0" t="s">
+      <c r="CD1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="CE1" s="0" t="s">
+      <c r="CE1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="CF1" s="0" t="s">
+      <c r="CF1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="CG1" s="0" t="s">
+      <c r="CG1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="CH1" s="0" t="s">
+      <c r="CH1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="CI1" s="0" t="s">
+      <c r="CI1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="CJ1" s="0" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="CK1" s="0" t="s">
+      <c r="CK1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="CL1" s="0" t="s">
+      <c r="CL1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="CM1" s="0" t="s">
+      <c r="CM1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="CN1" s="0" t="s">
+      <c r="CN1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="CO1" s="0" t="s">
+      <c r="CO1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="CP1" s="0" t="s">
+      <c r="CP1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="CQ1" s="0" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="CR1" s="0" t="s">
+      <c r="CR1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="CS1" s="0" t="s">
+      <c r="CS1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="CT1" s="0" t="s">
+      <c r="CT1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="CU1" s="0" t="s">
+      <c r="CU1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="CV1" s="0" t="s">
+      <c r="CV1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="CW1" s="0" t="s">
+      <c r="CW1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="CX1" s="0" t="s">
+      <c r="CX1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="CY1" s="0" t="s">
+      <c r="CY1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="CZ1" s="0" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="DA1" s="0" t="s">
+      <c r="DA1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="DB1" s="0" t="s">
+      <c r="DB1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="DC1" s="0" t="s">
+      <c r="DC1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="DD1" s="0" t="s">
+      <c r="DD1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="DE1" s="0" t="s">
+      <c r="DE1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="DF1" s="0" t="s">
+      <c r="DF1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="DG1" s="0" t="s">
+      <c r="DG1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="DH1" s="0" t="s">
+      <c r="DH1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="DI1" s="0" t="s">
+      <c r="DI1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="DJ1" s="0" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="DK1" s="0" t="s">
+      <c r="DK1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="DL1" s="0" t="s">
+      <c r="DL1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="DM1" s="0" t="s">
+      <c r="DM1" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="H2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>102</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="P3" s="0" t="s">
+      <c r="F3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="H3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="Q3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="S3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="T3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="V3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="W3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="X3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Y3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="BA3" s="0" t="s">
+      <c r="Z3" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="BB3" s="0" t="s">
+      <c r="BA3" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BC3" s="0" t="s">
+      <c r="BB3" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BD3" s="0" t="s">
+      <c r="BC3" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BE3" s="0" t="s">
+      <c r="BD3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="BF3" s="0" t="s">
+      <c r="BE3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="BH3" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="BI3" s="0" t="s">
+      <c r="BF3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="BJ3" s="0" t="s">
+      <c r="BH3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BI3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BK3" s="0" t="s">
+      <c r="BJ3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="BM3" s="0" t="s">
+      <c r="BK3" s="1" t="s">
         <v>126</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="D4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>132</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>